<commit_message>
Update experiment logic and params
- new condition span: 4-9
- allow responding while displaying the stimulus
</commit_message>
<xml_diff>
--- a/subitizing/practice_conditions.xlsx
+++ b/subitizing/practice_conditions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Dev\Psychopy\psychopy_experiments\subitizing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC85A7DD-4F74-4745-8A11-E9AA2880AC42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC6B80B-55A8-44C8-8774-C18D99A49518}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -348,10 +348,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -369,7 +369,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -377,7 +377,7 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -385,7 +385,7 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -393,7 +393,23 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>0.5</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>